<commit_message>
finish note spec, start related stuff
</commit_message>
<xml_diff>
--- a/argot/working_docs/notes_fields_table.xlsx
+++ b/argot/working_docs/notes_fields_table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="193">
   <si>
     <t>MARC tag</t>
   </si>
@@ -1622,7 +1622,7 @@
   <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3994,7 +3994,9 @@
       <c r="A42" s="4">
         <v>547</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>141</v>
       </c>

</xml_diff>